<commit_message>
Try to implement appending sheets
</commit_message>
<xml_diff>
--- a/sheeet.xlsx
+++ b/sheeet.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,41 +433,75 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>dr. Varga Krisztina</v>
+        <v>dr. Angyal Gabriella</v>
       </c>
       <c r="B4" t="str">
-        <v>1027 Budapest,Csalogány utca 21. I/3.</v>
+        <v>1036 Budapest,Árpád fejedelem útja 49. I/8.</v>
       </c>
       <c r="C4" t="str">
-        <v>+36 (1) 202 4276, +36 (1) 213 9433</v>
+        <v>+36 (1) 388 9603, +36 (1) 368 0267, +36 (1) 368 0266</v>
       </c>
       <c r="D4" t="str">
-        <v>vargakrisztina@mokk.hu, iroda.vk@kozjegyzo.hu</v>
+        <v>angyalg@mokk.hu</v>
       </c>
       <c r="E4" t="str">
-        <v>https:\\vargakrisztina.kozjegyzok.mokk.hu</v>
+        <v>https:\\angyalg.kozjegyzok.mokk.hu</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>dr. Szalontai Magdolna Rozália</v>
+        <v>dr. Steiner Erika Márta</v>
       </c>
       <c r="B5" t="str">
-        <v>1027 Budapest,Csalogány utca 7. I/1.</v>
+        <v xml:space="preserve">1034 Budapest,Kecske köz 12. </v>
       </c>
       <c r="C5" t="str">
-        <v>+36 (1) 225 3307, +36 (1) 225 3308</v>
+        <v>+36 (1) 387 5558, +36 (1) 250 3659</v>
       </c>
       <c r="D5" t="str">
-        <v>szalontai@mokk.hu</v>
+        <v>steiner.erika@mokk.hu</v>
       </c>
       <c r="E5" t="str">
-        <v>https:\\szalontai.kozjegyzok.mokk.hu</v>
+        <v>https:\\steinererika.kozjegyzok.mokk.hu</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>dr. Kertész Gabriella</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1033 Budapest,Miklós utca 11. III/12.</v>
+      </c>
+      <c r="C6" t="str">
+        <v>+36 (1) 388 9191, +36 (1) 388 2501</v>
+      </c>
+      <c r="D6" t="str">
+        <v>kertesz@mokk.hu</v>
+      </c>
+      <c r="E6" t="str">
+        <v>https:\\kertesz.kozjegyzok.mokk.hu</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>dr. Barbalics Miklós</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1036 Budapest,Árpád fejedelem útja 53/A. I/5.</v>
+      </c>
+      <c r="C7" t="str">
+        <v>+36 (1) 368 8305, +36 (1) 439 0670</v>
+      </c>
+      <c r="D7" t="str">
+        <v>barbalics@mokk.hu</v>
+      </c>
+      <c r="E7" t="str">
+        <v>https:\\barbalics.kozjegyzok.mokk.hu</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>